<commit_message>
made requested changes to formula, added fomatting for inCollections
</commit_message>
<xml_diff>
--- a/Invoice Manager.xlsx
+++ b/Invoice Manager.xlsx
@@ -441,10 +441,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L279"/>
+  <dimension ref="A1:L281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A277" sqref="A277:C294"/>
+    <sheetView tabSelected="1" topLeftCell="A266" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A278" sqref="A278:C288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -14097,50 +14097,72 @@
       </c>
     </row>
     <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>Written off</t>
+        </is>
+      </c>
       <c r="B274">
+        <f t="array" ref="B274">SUM(IF(F2:F273=FALSE,I2:I273,0))</f>
+        <v/>
+      </c>
+      <c r="C274" s="4">
+        <f>B274/B277</f>
+        <v/>
+      </c>
+      <c r="D274">
+        <f>SUM(I2:I36)</f>
+        <v/>
+      </c>
+      <c r="E274">
+        <f>SUMIFS(I2:I273,F2:F273,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Collected</t>
+        </is>
+      </c>
+      <c r="B275">
+        <f>SUMIFS(I2:I273,F2:F273,TRUE,K2:K273,"=0")</f>
+        <v/>
+      </c>
+      <c r="C275" s="4">
+        <f>B275/B277</f>
+        <v/>
+      </c>
+      <c r="D275">
+        <f>SUM(I37:I271)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="3" t="inlineStr">
+        <is>
+          <t>In Collections</t>
+        </is>
+      </c>
+      <c r="B276">
+        <f>SUMIFS(I2:I273,F2:F273,TRUE,K2:K273,"&lt;&gt;0")</f>
+        <v/>
+      </c>
+      <c r="D276">
+        <f>SUM(I272:I273)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>Total Billed</t>
+        </is>
+      </c>
+      <c r="B277">
         <f>SUM(I2:I273)</f>
         <v/>
       </c>
-      <c r="C274" t="inlineStr">
-        <is>
-          <t>billed</t>
-        </is>
-      </c>
-    </row>
-    <row r="275">
-      <c r="A275">
-        <f>B275/B274</f>
-        <v/>
-      </c>
-      <c r="B275">
-        <f>SUM(I2:I36)+SUM(I272:I273)</f>
-        <v/>
-      </c>
-      <c r="C275" t="inlineStr">
-        <is>
-          <t>write-off - not collected</t>
-        </is>
-      </c>
-    </row>
-    <row r="276">
-      <c r="A276" s="3" t="n">
-        <v>0.862815837</v>
-      </c>
-      <c r="B276">
-        <f>B274-B275</f>
-        <v/>
-      </c>
-    </row>
-    <row r="277">
-      <c r="A277" t="inlineStr">
-        <is>
-          <t>Total Billed</t>
-        </is>
-      </c>
-      <c r="B277">
-        <f>SUM(I2:I276)</f>
-        <v/>
-      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -14149,26 +14171,52 @@
         </is>
       </c>
       <c r="B278">
-        <f t="array" ref="B278">SUM(IF($F$2:$F$276=FALSE,$I$2:$I$276,0))+SUM(IF(K2:K276&lt;&gt;0,I2:I276,0))</f>
+        <f>SUMIFS(I2:I277,F2:F277,FALSE)</f>
         <v/>
       </c>
       <c r="C278" s="4">
-        <f>B278/B277</f>
+        <f>B278/B281</f>
         <v/>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t xml:space="preserve">Retiained </t>
+          <t>Collected</t>
         </is>
       </c>
       <c r="B279">
-        <f>B277-B278</f>
+        <f>SUMIFS(I2:I277,F2:F277,TRUE,K2:K277,"=0")</f>
         <v/>
       </c>
       <c r="C279" s="4">
-        <f>B279/B277</f>
+        <f>B279/B281</f>
+        <v/>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>In Collections</t>
+        </is>
+      </c>
+      <c r="B280">
+        <f>SUMIFS(I2:I277,F2:F277,TRUE,K2:K277,"&lt;&gt;0")</f>
+        <v/>
+      </c>
+      <c r="C280" s="4">
+        <f>B280/B281</f>
+        <v/>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>Total Billed</t>
+        </is>
+      </c>
+      <c r="B281">
+        <f>SUM(I2:I277)</f>
         <v/>
       </c>
     </row>

</xml_diff>